<commit_message>
Stop tracking .history cache
</commit_message>
<xml_diff>
--- a/electricity_calc_extra/Tarif_prices.xlsx
+++ b/electricity_calc_extra/Tarif_prices.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\fluttertwee\flutter\electricity_calc_extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A9ABBC-8076-4773-9C39-7EF740D980F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0609A086-EF8F-4351-A3DC-DE8C16CE1775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="20460" windowHeight="10770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -507,7 +507,7 @@
   <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,7 +636,7 @@
         <v>100</v>
       </c>
       <c r="G5">
-        <v>3.4258999999999999</v>
+        <v>1</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>19</v>
@@ -812,7 +812,7 @@
         <v>701</v>
       </c>
       <c r="G12">
-        <v>1.31558</v>
+        <v>13.155799999999999</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>22</v>

</xml_diff>